<commit_message>
Problems with gatex exergy calcultions from new formulation. Version of gatex seems to work coming from raw ebsilon input and from aspen input (without object oriented approach). In OO approach, something seems to be wrong with temperatures? TODO compare gatex output for exampleSim_aspen with example_exergyCalc01.
</commit_message>
<xml_diff>
--- a/example_exergyCalc01/ExampleSimulation.xlsx
+++ b/example_exergyCalc01/ExampleSimulation.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22221"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15620"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15620" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ExampleStreams1" sheetId="1" r:id="rId1"/>
     <sheet name="Examplestreams1_exergy" sheetId="2" r:id="rId2"/>
+    <sheet name="H2Ostreams" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="53">
   <si>
     <t>C3H6</t>
   </si>
@@ -188,10 +189,33 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -214,15 +238,36 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="11">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -517,11 +562,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="27" max="32" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="33" max="34" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="9.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:40">
       <c r="A1" s="1" t="s">
@@ -1484,6 +1561,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3200,4 +3278,128 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <f>273.15+15</f>
+        <v>288.14999999999998</v>
+      </c>
+      <c r="C2">
+        <v>1.0129999999999999</v>
+      </c>
+      <c r="D2">
+        <v>614.5</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>0.75043599999999999</v>
+      </c>
+      <c r="K2">
+        <v>0.22994000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <f>25+273.15</f>
+        <v>298.14999999999998</v>
+      </c>
+      <c r="C3">
+        <v>1.0129999999999999</v>
+      </c>
+      <c r="D3">
+        <v>65.209900000000005</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>833.78710000000001</v>
+      </c>
+      <c r="C4" s="3">
+        <v>124</v>
+      </c>
+      <c r="D4" s="3">
+        <v>65.209900000000005</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>